<commit_message>
pipeline and data analysis
</commit_message>
<xml_diff>
--- a/data/excelfiles/df_interresting_books.xlsx
+++ b/data/excelfiles/df_interresting_books.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,850 +436,1987 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>title</t>
+          <t>Titel</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>untertitel</t>
+          <t>Preis</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>autor</t>
+          <t>Autor</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>verlag</t>
+          <t>Genre</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>preis</t>
+          <t>Text</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>seiten</t>
+          <t>ISBN/GTIN</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>sprache</t>
+          <t>Produktart</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>einband</t>
+          <t>Einbandart</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>erscheinungsjahr</t>
+          <t>Verlag</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>artikelnummer</t>
+          <t>Erscheinungsdatum</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>isbn</t>
+          <t>Auflage</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>auflage</t>
+          <t>Reihe</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>reihe</t>
+          <t>Seiten</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>reihenbandnummer</t>
+          <t>Sprache</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>Masse</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Artikel-Nr.</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Die spürst du nicht </t>
+          <t>Der Feind</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>24.90</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Glattauer, Daniel</t>
+          <t>Brand, Christine</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Zsolnay</t>
+          <t>belletristik krimi</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CHF 34.50</t>
+          <t>Ein bizarre Mordserie an Männern sowie Schüsse während einer Frauendisko - in Band 5 der Erfolgsserie halten gleich zwei Fälle Milla Nova und das Team um Sandro Bandini auf Trab.
+Ein bizarrer Mord sorgt für Aufsehen: Ein Mann wurde an sein Bett gefesselt und hingerichtet. An den Füßen trägt er rote Stöckelschuhe. Schnell stellt sich heraus, dass er zuvor eine Drohung erhielt: ein Foto von sich selbst - mit dem Absatz eines Stöckelschuhs im Gesicht. Er ist nicht der Einzige, der solch eine Nachricht bekam. Sind auch die anderen Bedrohten in Gefahr? Gleichzeitig jagt das Team um Polizeichef Sandro Bandini einen Mann, der in einer Frauendisko in einem linken Kulturzentrum um sich schoss. Die Vermutung eines rechtsextremen Hintergrunds liegt nahe, doch TV-Reporterin Milla Nova vermutet ein anderes Motiv: Frauenhass. Gemeinsam mit ihrem blinden Freund Nathaniel taucht sie in die dunkle Welt der Incels ein. Zwei Fälle, bei denen der Hass auf das andere Geschlecht eine vitale Rolle spielt. Ist es Zufall oder besteht ein Zusammenhang?
+Die unabhängig voneinander lesbaren Krimis um Milla Nova und Sandro Bandini:
+1. Blind
+2. Die Patientin
+3. Der Bruder
+4. Der Unbekannte
+5. Der Feind
+Lesen Sie auch »Wahre Verbrechen»: Christine Brand schreibt über ihre dramatischsten Fälle als Gerichtsreporterin.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>304 S.</t>
+          <t>978-3-7645-0771-8</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Fester Einband</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Blanvalet</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>42421530</t>
+          <t>26.04.2023</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>978-3-552-07333-3</t>
+          <t>1. A.</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>n-Nr.05</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Der Bestsellerautor Daniel Glattauer lässt in seinem neuen Roman Menschen zu Wort kommen, die keine Stimme haben - ein Sittenbild unserer privilegierten Gesellschaft. Die Binders und die Strobl-Marineks gönnen sich einen exklusiven Urlaub in der Toskana. Tochter Sophie Luise, 14, durfte gegen die Langeweile ihre Schulfreundin Aayana mitnehmen, ein Flüchtlingskind aus Somalia. Kaum hat man sich mit Prosecco und Antipasti in Ferienlaune gechillt, kommt es zur Katastrophe. Was ist ein Menschenleben wert? Und jedes gleich viel? Daniel Glattauer packt große Fragen in seinen neuen Roman, den man nicht mehr aus der Hand legen kann und in dem er all sein Können ausspielt: spannende Szenen, starke Dialoge, Sprachwitz. Dabei zeichnet Glattauer ein Sittenbild unserer privilegierten Gesellschaft, entlarvt deren Doppelmoral und leiht jenen seine Stimme, die viel zu selten zu Wort kommen.</t>
-        </is>
-      </c>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sommerschwestern - Die Nacht der Lichter </t>
+          <t>Elternabend</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>23.90</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Peetz, Monika</t>
+          <t>Fitzek, Sebastian</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Kiepenheuer &amp; Witsch</t>
+          <t>belletristik romane</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CHF 23.90</t>
+          <t>Stell dir vor ...
+... du musst eine halbe Ewigkeit auf einem Elternabend verbringen. Dabei hast du gar kein Kind!
+Ein lebenskluger und hinreißend komischer Roman im Stil von Sebastian Fitzeks Nr.1-Bestseller »Der erste letzte Tag«
+Sascha Nebel hat sich zur falschen Zeit am falschen Ort das falsche Auto für einen Diebstahl ausgesucht. Kaum, dass er hinter dem Steuer eines Geländewagens Platz genommen hat, zieht eine Horde demonstrierender Klimaaktivisten durch die Straße. Allen voran eine junge Frau, die den SUV mit einer Baseballkeule demoliert. Als die Polizei auf der Bildfläche erscheint, ergreifen Sascha und die Unbekannte die Flucht und platzen in den Elternabend einer 5. Klasse. Um die Nacht nicht in Polizeigewahrsam zu verbringen, bleibt ihnen keine andere Wahl: Sie müssen in die Rolle von Christin und Lutz Schmolke schlüpfen, den Eltern des 11jährigen Hector, die bislang jede Schulveranstaltung versäumten. Zwei wildfremde Menschen, zwischen denen kaum größeres Streitpotential herrschen könnte, geben sich als Vater und Mutter eines ihnen völlig unbekannten Kindes aus. Dabei ist die Tatsache, dass Hector der größte Rüpel der Schule ist, sehr schnell ihr kleinstes Problem ...</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>352 S.</t>
+          <t>978-3-426-28413-1</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Droemer/Knaur</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>42779092</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>978-3-462-00398-7</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>1. Auflage</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Die Sommerschwestern-Romane</t>
-        </is>
-      </c>
+          <t>26.04.2023Erstverkaufstag26.04.2023</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Monika Peetz' vier »Sommerschwestern« kehren zurück an ihren Ferienort Bergen an der holländischen Nordseeküste, auf der Spur des großen Familiengeheimnisses. Eine spannende Suche nach der Wahrheit über den Tod ihres Vaters vor sommerlicher Urlaubskulisse. </t>
-        </is>
-      </c>
+          <t>Breite 135 mm, Höhe 210 mm, Dicke 25 mm</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bündner Sturm </t>
+          <t>Das Café ohne Namen</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ein Fall für Giulia de Medici</t>
+          <t>34.90</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Gurt, Philipp</t>
+          <t>Seethaler, Robert</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Kampa Verlag</t>
+          <t>belletristik romane</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CHF 24.90</t>
+          <t>Ein Café und seine Menschen. Ein Mann, der seiner Sehnsucht folgt. Robert Seethalers neuer Roman.
+Wien im Jahr 1966. Robert Simon verdient sein Brot als Gelegenheitsarbeiter auf dem Karmelitermarkt. Er ist zufrieden mit seinem Leben, doch zwanzig Jahre nach Ende des Krieges hat sich die Stadt aus ihren Trümmern erhoben. Überall wächst das Neue, und auch Simon lässt sich mitreißen. Er pachtet eine Gastwirtschaft und eröffnet sein eigenes Café. Das Angebot ist überschaubar, und genau genommen ist es gar kein richtiges Café, doch die Menschen aus dem Viertel kommen, und sie bringen ihre Geschichten mit - von der Sehnsucht, vom Verlust, vom unverhofften Glück. Sie kommen auf der Suche nach Gesellschaft, manche hoffen sogar auf die Liebe, und während die Stadt um sie herum erwacht, verwandelt sich auch Simons eigenes Leben.
+Das Café ohne Namen ist ein Roman über den menschlichen Drang zum Aufbruch. Mit einem Reigen unvergesslicher Figuren und seiner besonderen Aufmerksamkeit für die Details des Lebens erzählt Robert Seethaler davon, wie eine neue Welt entsteht, die wie alles Neue ihr Ende schon in sich trägt.
+"Niemand muss Robert Seethaler lesen, um zu begreifen, dass das Scheitern die zentrale Erfahrung des Lebens ist. Aber man liest davon bei Seethaler nach wie vor lieber als anderswo, weil er so behutsam davon zu erzählen versteht, ohne größere Ausflüchte oder Umwege." Cornelius Pollmer, Süddeutsche Zeitung</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>336 S.</t>
+          <t>978-3-546-10032-8</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>42907560</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>978-3-311-12060-5</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Ein Fall für Giulia de Medici</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
-      </c>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Ein Sturm zieht über das herbstlich gefärbte Engadin, als Giulia de Medici, Alpinpolizistin und Chefermittlerin der Kantonspolizei Graubünden, zu einer Leiche auf den Roseggletscher gerufen wird. Dort angekommen, ist Giulias Verwunderung groß: Die fast gänzlich eingefrorene Tote trägt ein rotes Sommerkleid, und die zum Fundort gerufene Forensikerin stellt fest, dass die junge Frau bereits vor über zwanzig Jahren ermordet wurde. Als Giulia auf dem Weg zurück ins Tal in der Berghütte Chamanna Coaz Rast macht und dabei auch noch auf die tote Hüttenwartin stößt, beginnt eine aufreibende Jagd nach den Schuldigen. Liebe, Verrat, Leidenschaft und Intrigen zwingen die temperamentvolle Berglerin beinahe in die Knie.</t>
-        </is>
-      </c>
+          <t>Breite 128 mm, Höhe 210 mm, Dicke 28 mmGewicht386 g</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Windhauch, das ist alles Windhauch </t>
+          <t>Mit dem Mut zur Liebe</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>19.90</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ryser, Werner</t>
+          <t>Lind, Hera</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Cosmos</t>
+          <t>taschenbuch romane</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CHF 36.00</t>
+          <t>Erst ein dramatischer Unfall, dann die waghalsige Flucht aus der DDR:
+Im Tatsachenroman »Mit dem Mut zur Liebe« erzählt Nummer-1-Bestseller-Autorin Hera Lind die wahre Liebesgeschichte der Artisten Dieto und Johanna.
+Es ist Liebe auf den ersten Blick, als sich Johanna und Dieto 1957 in Dresden zum ersten Mal begegnen. Ihre Väter waren zusammen in russischer Kriegsgefangenschaft, und beide bringen ihren Kindern die artistischen Kunststücke bei, die ihnen den sicheren Tod im Arbeitslager erspart haben. Doch als das junge Artistenpaar nach hartem Drill schließlich Weltniveau erreicht, muss Dieto sich drei Jahre beim Militär verpflichten. Das junge Paar flieht Hals über Kopf in einem Schlauchboot über die Adria, wo sie nur mit Badesachen bekleidet nach 36 Stunden völlig erschöpft ankommen .Da wird ihnen bewusst, dass sie ohne ihr Equipmentkeine Existenz aufbauen können. Dieto lässt Johanna bei Fremden zurück und versucht es ein zweites Mal....
+Ergreifend und voller Hoffnung erzählt der dramatische Tatsachenroman von Bestseller-Autorin Hera Lind die wahre Geschichte eines ganz normalen Paares aus der DDR, dessen Liebe über alle Grenzen trägt.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>272 S.</t>
+          <t>978-3-426-52840-2</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Taschenbuch</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Fester Einband</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Droemer/Knaur</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>43216342</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>978-3-305-00492-8</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>02.05.2023</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>«Jetzt kehre ich als Bettler dorthin zurück, wo man Vater um sein Erbe betrogen hat.» Am 18. Juli 1930 verlässt Hannes mit seiner Familie Georgien, das Land, in dem er geboren wurde. Simon, sein Vater, war 1866 in Langnau im Emmental aufgebrochen, um in Grusinien, wie die Russen Georgien nannten, seinen Traum zu verwirklichen: ein Geschlecht von angesehenen Bauern zu gründen. Als Simon 1918 starb, hinterliess er Hannes einen Gutshof mit mehr als tausend Kühen. Doch nach dem Einmarsch der Roten Armee und der Machtübernahme der Bolschewiki in Transkaukasien verliert die Familie ihren ganzen Besitz. Die Schweizer Auswanderer dürfen nicht mehr mitnehmen, als in einem Koffer Platz hat. Und sie haben noch Glück: Die deutschen Kolonisten werden deportiert - viele von ihnen verlieren in Sibirien ihr Leben. Der letzte Band von Werner Rysers kaukasischer Tetralogie hat beklemmende Parallelen zu aktuellen Ereignissen auf der Welt. Es scheint, als wiederhole sich die Geschichte. Immer wieder. «Kaukasische Sinfonie» ist der dritte Band einer Familiensaga, die mit den Romanen «Geh, wilder Knochenmann!» und «Die grusinische Braut» begonnen hat. Der Roman spielt vor dem Hintergrund weltgeschichtlicher Ereignisse: des Grossen Kriegs von 1914/18 und der Russischen Revolution, die das Schicksal der Menschen im kleinen Land zwischen dem Schwarzen und dem Kaspischen Meer prägen.</t>
-        </is>
-      </c>
+          <t>Breite 125 mm, Höhe 190 mm, Dicke 36 mmGewicht441 g</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bretonische Idylle </t>
+          <t>Gnadenlose Provence</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Kommissar Dupins zehnter Fall</t>
+          <t>25.90</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Bannalec, Jean-Luc</t>
+          <t>Lagrange, Pierre</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Kiepenheuer &amp; Witsch</t>
+          <t>belletristik krimi</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CHF 18.50</t>
+          <t>Eine gnadenlose Tat erschüttert die Provence - der achte Band der Provence-Krimi-Reihe von Bestseller-Autor Pierre Lagrange
+Zahllose Radsportler sausen im Sommer durch die Provence - und ein Scharfschütze zieht einen nach dem anderen aus dem Verkehr. Die Ermittler Castel und Theroux sind geschockt und haben keinen Schimmer, um wen es sich bei dem Täter handeln könnte. Albin Leclerc, Commissaire im Ruhestand, erfährt von den Vorfällen, während er seine Flitterwochen auf Martinique verbringt. Kaum zurück, stürzt er sich in die Ermittlungen. Er befürchtet, dass der Schütze sich bisher nur aufwärmt und es auf die Tour de France abgesehen hat, die in Kürze durch Carpentras führen wird. Ein Rennen um Leben und Tod beginnt, bei dem sich herausstellt: Die Hintergründe sind finsterer als gedacht ...
+Ex-Commissaire Albin Leclerc ermittelt in der Provence: die Provence-Krimi-Reihe
+Band 1: Tod in der Provence
+Band 2: Blutrote Provence
+Band 3: Mörderische Provence
+Band 4: Schatten der Provence
+Band 5: Düstere Provence
+Band 6: Eiskalte Provence
+Band 7: Trügerische Provence
+Band 8: Gnadenlose Provence
+Band 9: Unheilvolle Provence</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>336 S.</t>
+          <t>978-3-651-02592-9</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>FISCHER Scherz</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>42779812</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>978-3-462-00489-2</t>
-        </is>
-      </c>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>1. Auflage</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Kommissar Dupin ermittelt</t>
-        </is>
-      </c>
+          <t>n-Nr.08</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>Malerische Abgründe - Kommissar Dupin ermittelt auf der legendären Belle-Île.</t>
-        </is>
-      </c>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Stumme Schreie </t>
+          <t>Provenzalische Täuschung</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Flint &amp; Cavalli ermitteln hinter verschlossenen Türen. Kriminalroman. Ein Fall für Flint und Cavalli (9)</t>
+          <t>25.90</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ivanov, Petra</t>
+          <t>Bonnet, Sophie</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Unionsverlag</t>
+          <t>belletristik krimi</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CHF 22.00</t>
+          <t>Aromatische Trüffel, grüne Eichenwälder und ein toter Polizist - ein neuer Fall für den liebeswerten Ermittler Pierre Durand!
+Es ist Trüffelzeit in der Provence. Pierre und Charlotte bereiten ihre Hochzeit vor, als eine Nachricht Sainte-Valérie in Aufregung versetzt: Gilbert Langlois - kürzlich in das Bergdorf gezogen, um Pierre seinen Posten streitig zu machen - liegt tot im Bach. Der Verdacht fällt auf Pierre, doch der glaubt zu wissen, wer der wahre Täter ist: Maurice Marechal, der Bürgermeister des Ortes. Fest entschlossen, ihn des Mordes zu überführen, beginnt Pierre verdeckt zu ermitteln. Die Spur führt ihn nach Mazan unweit des Mont Ventoux, wo sowohl das Opfer als auch Marechal aufgewachsen sind, und zu einem tragischen Fall aus der Vergangenheit. Alles deutet darauf hin, dass beide Geschehnisse miteinander verknüpft sind, als Pierre feststellt, dass es eine Person gibt, die sich an seine Fersen geheftet hat ...
+»Niemand verbindet Genuss und Verbrechen so harmonisch wie Sophie Bonnet in ihren Provence-Krimis.« Hamburger Morgenpost</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>352 S.</t>
+          <t>978-3-7645-0792-3</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Blanvalet</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>42890567</t>
+          <t>11.05.2023</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>978-3-293-20952-7</t>
+          <t>Originalausgabe</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Ein Fall für Flint &amp; Cavalli; Unionsverlag Taschenbücher; metro</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>n-Nr.09</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>Bruno Cavalli und Regina Flint stehen vor ganz neuen Herausforderungen. Cavalli kehrt nach langem Aufenthalt in den USA in die Schweiz zurück und tritt eine neue Stelle an. Dort wartet eine heikle Aufgabe auf ihn: Er soll einen Vorwurf gegen einen Polizisten untersuchen.</t>
-        </is>
-      </c>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Die Rebellin und der Dieb </t>
+          <t>Das Leuchten von Lavendel</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>17.90</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Sendker, Jan-Philipp</t>
+          <t>Luis, Hannah</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Heyne Taschenb.</t>
+          <t>taschenbuch romane</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CHF 16.90</t>
+          <t>Duftender Lavendel und die verführerischen Genüsse der Provence
+Mit einem ihrer selbst gebackenen Kuchen will Emilia ihren trauernden Großvater auf andere Gedanken bringen. Doch dann findet sie in seinem Keller einen alten Brief mit einer französischen Adresse und einem Herz aus Lavendelblüten, das den Namen Jette umrankt. Von einer Jette hat jedoch noch nie jemand aus der Familie gehört. Ihr Opa weigert sich, darüber zu sprechen. Also reist Emilia in die Provence, um nach der Unbekannten zu suchen. Sie hilft bei der Ernte auf der Lavendelfarm, auf der bereits ihr Großvater in jungen Jahren gearbeitet hat. Verzaubert vom magischen Licht und dem verführerischen Duft, kommt Emilia dem Rätsel des Lavendelherzens schließlich auf die Spur. Als sie dem attraktiven Besitzer der benachbarten Farm begegnet, muss sie sich jedoch fragen, warum ihr eigenes Herz plötzlich schneller schlägt.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>320 S.</t>
+          <t>978-3-453-42737-2</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Taschenbuch</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Heyne</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>38616351</t>
+          <t>11.05.2023</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>978-3-453-42706-8</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Erstmals im TB</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>Originalausgabe</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Die universelle Geschichte zweier Liebender aus verschiedenen Welten, die lernen, was im Angesicht einer Katastrophe zählt: Mut zum Widerstand, Wille zur Veränderung und bedingungsloses Vertrauen ineinander.</t>
-        </is>
-      </c>
+          <t>Breite 119 mm, Höhe 187 mm, Dicke 36 mmGewicht381 g</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sommerschwestern </t>
+          <t>Wenn jeder dich mag, nimmt keiner dich ernst</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Roman | Der SPIEGEL-Bestseller #1 von der Autorin der »Dienstagsfrauen«</t>
+          <t>26.90</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Peetz, Monika</t>
+          <t>Wehrle, Martin</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Kiepenheuer &amp; Witsch</t>
+          <t>fachbuecher psychologie psychologie</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>CHF 16.90</t>
+          <t>Sagen Sie zu selten, was Sie wirklich wollen?
+Wie oft sagen Sie, was tatsächlich in Ihnen vorgeht? Und wie oft behalten Sie Ihre Meinung für sich, aus Sorge, anderen damit auf den Schlips zu treten? Wer alles tut, was andere von ihm wollen, ist zwar beliebt - aber lediglich als leichtes Opfer. Nur wem es gelingt, sich nicht verunsichern zu lassen und auch unbequeme Haltungen zu vertreten, wird die eigenen Ziele erreichen. Bestseller-Autor Martin Wehrle zeigt, wie Sie in jeder Lebenslage Ihre Selbstachtung verteidigen.
+Für alle, die
+_ sich nicht länger ausnutzen lassen wollen,
+_ ihren Willen durchsetzen möchten,
+_ souverän kontern wollen, wenn ihr Gegenüber sie überfordert, kleinmacht oder angreift.
+Ein Buch voller Kraft und Inspiration, das Sie selbstbewusster und schlagfertiger macht!</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>304 S.</t>
+          <t>978-3-442-39409-8</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Mosaik</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>42780273</t>
+          <t>26.04.2023</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>978-3-462-00447-2</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>1. Auflage</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>Die Sommerschwestern-Romane</t>
-        </is>
-      </c>
+          <t>Originalausgabe</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Vier erwachsene Schwestern, die unterschiedlicher nicht sein könnten, folgen der rätselhaften Einladung ihrer kapriziösen Mutter zu einem Familientreffen am Ferienort ihrer Kindheit. Mit gemischten Gefühlen treffen sie im malerischen Örtchen Bergen an der holländischen Küste ein. Jede mit ihren eigenen Sorgen und Gedanken im Gepäck. Warum ruft die Mutter sie zusammen? </t>
-        </is>
-      </c>
+          <t>Breite 139 mm, Höhe 207 mm, Dicke 31 mmGewicht421 g</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Das Glück in den Wäldern </t>
+          <t>Am Horizont wartet die Sonne</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ein Sehnsuchtswald-Roman</t>
+          <t>17.90</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Koelle, Patricia</t>
+          <t>Werkmeister, Meike</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Fischer Taschenb.</t>
+          <t>taschenbuch romane</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>CHF 16.90</t>
+          <t>Der große neue Sommerroman der SPIEGEL-Bestsellerautorin
+Es gibt keine Zufälle, es gibt nur Zeichen. Davon ist die Hamburger Autorin Katrin überzeugt. Doch während sie Bücher schreibt, die anderen Orientierung geben sollen, steckt sie selbst in einer Lebenskrise. Bis das Schicksal auch ihr ein Zeichen gibt: Als sie einen Liebesbrief findet, adressiert an einen Filipe in Portugal, beschließt sie, dem Empfänger die Botschaft persönlich zu überbringen. Mit ihrer Freundin Julia reist sie auf eine idyllische Halbinsel an der Atlantikküste, die Heimat des geheimnisvollen Filipe. Bei der Suche nach ihm gerät Katrin unversehens in ein Familiendrama. Und findet etwas, wonach sie gar nicht gesucht hat ...</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>496 S.</t>
+          <t>978-3-442-49416-3</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Taschenbuch</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Goldmann</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>42091910</t>
+          <t>03.05.2023</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>978-3-596-70723-2</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>1. Auflage</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Sehnsuchtswald-Reihe</t>
-        </is>
-      </c>
+          <t>1. A.</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manchmal führt der Weg zum Glück durch einen geheimnisvollen Wald - der zweite Band der Sehnsuchtswald-Reihe von Bestseller-Autorin Patricia Koelle </t>
-        </is>
-      </c>
+          <t>Breite 126 mm, Höhe 188 mm, Dicke 29 mmGewicht368 g</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hotel Freiheit </t>
+          <t>Das größte Glück im Leben</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Sylt-Saga 3 - Roman</t>
+          <t>24.90</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>Hauptmann, Gaby</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Töpferin Maike kämpft um ihre Existenz und ihr Elternhaus in Timmendorfer Strand
+Maike liebt ihr kleines, von Rosen umranktes Elternhaus in Timmendorfer Strand. Und obwohl es komisch klingt, fühlt sie, dass auch das Haus sie liebt. Seit ihrer Trennung lebt sie dort allein in einer idyllischen Sackgasse. Nicht ganz allein, denn mit ihren Nachbarn bildet sie eine verschworene Gemeinschaft. Bis ein Immobilienmakler ein Auge auf ihr Häuschen wirft - ihm ist jedes Mittel recht, um sein Ziel zu erreichen. Und er scheint zu wissen, dass Maike als Töpferin kaum Einnahmen hat ... Wie aus einem vermeintlichen Unglück Glück entstehen kann, erzählt niemand besser als Gaby Hauptmann!</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>978-3-492-06460-6</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Piper</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Breite 136 mm, Höhe 205 mm, Dicke 32 mmGewicht452 g</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>55179762</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Die Tote im Luganer See</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>26.90</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Vassena, Mascha</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>belletristik krimi</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Im beschaulichen Luganer See wird eine Leiche gefunden, und die Tote ist niemand Geringeres als die einst berühmte Chansonsängerin Livia. Doch wer hatte einen Grund, die alte, zurückgezogen lebende Dame zu töten? Wieder bitten Jugendliebe und Leiter der örtlichen Gerichtsmedizin Luca Cavadini und Ispettrice Moretti die Dolmetscherin Moira Rusconi bei dem Fall um Unterstützung. Die Ermittlungen führen sie in ein Geflecht aus dubiosen Geschäften, Rachegelüsten und Familiengeheimnissen. Und während ihr Vater Ambrogio sich in der Casa Rusconi mit ihrer anspruchsvollen Mutter abmüht, stellt Moira eigenmächtig Nachforschungen an und bringt sich dabei unwissentlich in Lebensgefahr.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>978-3-8479-0134-1</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Eichborn</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>28.04.2023</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>1. Aufl. 2023</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>n-Nr.02</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Liebe oder Eierlikör - Fast eine Romanze</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>23.90</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Heldt, Dora</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Früher war mehr Romantik ...
+Ernst Mannsen versteht die Welt nicht mehr. Die sonst so verlässliche Hilke Petersen trägt plötzlich Lippenstift und hat keine Zeit, auf dem Frühlingsbazar Kuchen zu verkaufen. Hella und Gudrun reden von Frühlingsgefühlen und Liebeshormonen und vermuten, dass Hilke eine Romanze hat. Und plötzlich taucht auch noch das Gerücht auf, dass das halbe Dorf sich bei einer Dating-App angemeldet hat, die Liebe oder Eierlikör heißt. Und das, obwohl Ernst schon so viel über Betrüger im Netz gelesen hat. Er vermutet, dass der Lippenstift nur der Anfang der Katastrophe ist, in die Hilke sich begibt, und ist entschlossen, das zu verhindern. Mithilfe seines Enkels Mats und Freundin Hella forscht er undercover nach, nicht ahnend, wie schnell man sich auf einem Date wiederfinden kann ...</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>978-3-423-28337-3</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>DTV</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Breite 119 mm, Höhe 175 mm, Dicke 24 mmGewicht280 g</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Der kleine Drache Kokosnuss - Aufregung in der Drachenschule</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>15.90</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Siegner, Ingo</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>kids ersteslesen</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Ein Schulfach namens »Abenteuer«
+In der Drachenschule bespricht Dr. Blumenkohl die Tiere, die es früher auf der Dracheninsel gab. Als Kokosnuss erzählt, dass auch der »dreiköpfige Höhlendrache« hier gelebt hat, wird er von allen ausgelacht. Der Höhlendrache sei doch nur eine Fabelfigur aus Kokosnuss' Lieblings-Piratengeschichte!Doch Kokosnuss glaubt fest daran, dass jede Geschichte einen wahren Kern hat. Jetzt will er forschen und beweisen, dass es die Höhlendrachen wirklich gab. Natürlich lassen ihn Oskar und Matilda auch bei diesem Abenteuer nicht im Stich ...
+Die Geschichten über die aufregenden Abenteuer, die der kleine Drache Kokosnuss mit seinen Freunden erlebt, sind inzwischen wahre Kinderbuchklassiker. Ingo Siegner schreibt über Freundschaft und Mut und fügt originelle Illustrationen hinzu. Die »Dein Spiegel-Bestseller-Reihe« eignet sich perfekt zum Vor- und Selberlesen.
+Ausstattung: Mit fbg. Illustrationen</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>978-3-570-18068-6</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>cbj</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>11.05.2023</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Originalausgabe</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>n-Nr.31</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Flugzeuge der Welt 2023</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>22.90</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Müller, Claudio</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>freizeit fahrzeuge verkehr</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Auch 2023 werden in diesem Standardwerk wieder Flugzeugmuster vorgestellt, die derzeit erprobt werden, sich in Produktion befinden, oder voraussichtlich 2023 ihren Erstflug absolvieren. Die verschiedenen Modelle werden in bewährter Art in Bild, Text und Dreiseitenrissen dargestellt und erläutert. Schwerpunktthema der 63. Ausgabe werden Drohnen sein - in militärischen Konflikten gewinnen sie immer mehr an Bedeutung. Auch ältere russische Flugzeugtypen werden vorgestellt, die durch die westlichen Sanktionen in Russland derzeit wieder stark nachgefragt sind. Somit wird auch in Flugzeuge der Welt 2023 wieder für Abwechslung gesorgt.</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>978-3-613-04528-6</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>25.04.2023</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Breite 100 mm, Höhe 165 mm, Dicke 20 mmGewicht352 g</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>55694935</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Trügerische Provence</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>17.90</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Lagrange, Pierre</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>taschenbuch krimis</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Ein trügerischer Festspiel-Sommer in der Provence - der siebte Band der Provence-Krimi-Reihe von Bestseller-Autor Pierre Lagrange
+Mitten in der Konzertsaison in der Provence verschwinden plötzlich namhafte Musikerinnen. Die Ermittlungskommission unter Leitung von Caterine Castel und Alain Theroux tappt im Dunkeln. Es gibt keine Hinweise oder Forderungen im Zusammenhang mit der Entführung. Obwohl Ex-Commissaire Albin Leclerc mitten in den eigenen Hochzeitsvorbereitungen steckt, kann er es mal wieder nicht lassen: zusammen mit seinem Mops Tyson nimmt er die Spur auf. Als es zu einer weiteren Entführung kommt, und auch die kostbaren Instrumente verschwinden, stellt sich für ihn die Frage, ob in der Provence ein Wahnsinniger unterwegs ist. Die Ermittlungen bringen Albin Leclerc in allergrößte Gefahr ...</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>978-3-596-70646-4</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Taschenbuch</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>FISCHER Taschenbuch</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>n-Nr.07</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Die Wikingerin</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>26.90</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Glaesener, Helga</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>belletristik historische</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Solvejg - eine Wikingerin auf der Flucht
+Solvejg ist eine junge Wikingerin. Ihr Vater, König Harald Schönhaar, glaubt, von seiner toten Frau verzaubert worden zu sein, und gibt seiner Tochter die Schuld daran. Solvejg muss fliehen. In Männerkleidern heuert sie bei fremden Wikingern an, die auf einen Raubzug nach Irland wollen. Doch die Norweger werden besiegt, und sie wird eingekerkert - zusammen mit Dhoire, einem Druiden, der sich mit Magie und Mathematik befasst und der sie in einer Nacht verführt. Schwanger gelingt Solvejg die Flucht ins Reich der Franken, aber sie hat mächtige Verfolger: Dhoire, der fürchtet, sie könnte hinter seine Geheimnisse der Magie gekommen sein - und ein Mann namens Einar Schlangenauge. Der Wikinger hat von König Harald einen mörderischen Auftrag bekommen. Er soll ihm den Kopf seiner Tochter bringen.
+Ein großes historisches Abenteuer: eine junge Frau und ihre Flucht durch halb Europa.
+Für Fans von "Game of Thrones" und "Vikings"</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>978-3-352-00962-4</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Rütten &amp; Loening</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>18.04.2023</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Breite 135 mm, Höhe 215 mm, Dicke 34 mmGewicht483 g</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Pferdeflüsterer-Academy, Band 12: Wild und verwundbar</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>19.90</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Mayer, Gina</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>kids bis11</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Im wilden Kanada steht ein weißes Schloss: Snowfields. Auf dem Internat werden die weltbesten Reiter ausgebildet und verletzte Pferdeseelen geheilt.
+Zwei Neue in Snowfields sorgen für Liebeschaos pur. Der attraktive Schüler Petter, zu dem sich Zoes Freundin Isabelle stark hingezogen fühlt. Und die junge Lehrerin, die bei einigen Lehrkräften heftigste Gefühle auslöst. Doch auch auf anderer Ebene herrscht Chaos. Im Internet kursieren schlimme Gerüchte über den Pferdeflüsterer Caleb. Und so langsam beschleicht Zoe das Gefühl, dass das nicht alles nur Lügen sind ...
+Entdecke alle Abenteuer an der "Pferdeflüsterer-Academy":
+Band 1: Reise nach Snowfields
+Band 2: Ein geheimes Versprechen
+Band 3: Eine gefährliche Schönheit
+Band 4: Verletztes Vertrauen
+Band 5: Zerbrechliche Träume
+Band 6: Calypsos Fohlen
+Band 7: Flammendes Herz
+Band 8: Zoes größter Sieg
+Band 9: Cyprians Rückkehr
+Band 10: Die dunkle Wahrheit</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>978-3-473-40461-2</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>01.05.2023</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>1. Aufl.</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>HC - Pferdeflüsterer-Academy</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Breite 147 mm, Höhe 216 mm, Dicke 24 mm</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Adas Fest</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>32.90</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Burseg, Katrin</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Ein großer Roman über Festhalten und Loslassen von Familie
+Ein Strandhaus an der französischen Atlantikküste mitten im Sommer. Doch der schöne Schein trügt. Der ansteigende Meeresspiegel verschlingt die Küste, und auch 'Les Vagues', an das die 74-jährige Ada vor vielen Jahren ihr Herz verloren hat, droht bei einem der nächsten Herbststürme ins Meer zu kippen. Ein letztes Mal noch möchte Ada ein rauschendes Fest feiern: in Erinnerung an ihren Mann, den berühmten Maler Leo Kwant, zusammen mit ihren Kindern, Freunden von früher und Vincent, dem Restaurantbesitzer aus dem Ort. Als die erwachsenen Töchter mit eigenen Sorgen anreisen, entgeht ihnen zunächst, dass Ada und Vincent etwas verbindet, das mit der Vergangenheit zu tun hat. Doch was Ada all die Jahre vor ihnen verheimlicht hat, ist so aufwühlend und tiefgreifend zugleich - es wird ihrer aller Leben für immer verändern.</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>978-3-453-29223-9</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Diana</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Originalausgabe</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Breite 136 mm, Höhe 206 mm, Dicke 35 mmGewicht474 g</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Vor uns das Leben</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>26.90</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Inusa, Manuela</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>jugend junge_erwachsene</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Auf der Reise durch die USA zur ersten großen Liebe!
+Als ihr Vater bei einem Unfall ums Leben kommt, bricht für die 17-jährige Alice eine Welt zusammen. Monatelang zieht sie sich in ihr Schneckenhaus zurück. Bis sie einen Stapel alter Briefe ihrer Mutter findet, welche die Familie vor Jahren verlassen hat. Alice beschließt, ihre Mutter zu suchen. Mit dem alten Auto ihres Vaters macht sie sich auf den langen Weg durch den Westen der USA. Und dort, auf einsamen Highways, in wunderschönen Nationalparks und aufregenden Städten findet Alice schließlich nicht nur zu sich selbst, sondern auch ihre erste große Liebe.</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>978-3-499-00808-5</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Rowohlt TB.</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>18.04.2023</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Breite 140 mm, Höhe 215 mm, Dicke 25 mmGewicht365 g</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Man vergisst nicht, wie man schwimmt</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>19.90</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Huber, Christian</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>taschenbuch romane</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>»Die einzige Möglichkeit, etwas vom Leben zu haben, ist, sich hineinzuwerfen.«
+31. August 1999. Sengende Hitze liegt über Bodenstein, dem Heimatkaff des 15-jährigen Pascal. Es sind die großen Ferien, und eigentlich könnte der Junge den Sommer genießen. Den Skatepark. Die Partys der Oberstufler. Das Freibad mit den besten Pommes des Planeten. Doch seit er nicht mehr schwimmen kann, mag Pascal den Sommer nicht mehr. Warum das so ist, das kann er nicht erzählen. Ebenso wenig, wieso ihn alle Krüger nennen. Und erst recht nicht, warum er sich unter keinen Umständen verlieben darf. Lieber träumt er vor sich hin und schreibt Geschichten. Dann kracht Jacky in seine Welt. Ein geheimnisvolles Mädchen aus dem Zirkus. Mit roten Haaren, wasserblauen Augen und keiner Angst vor nichts. Zusammen verbringen sie einen flirrenden, letzten Sommertag, der alles für immer verändert ...</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>978-3-423-21856-6</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Taschenbuch</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>DTV</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Breite 122 mm, Höhe 191 mm, Dicke 29 mmGewicht329 g</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Herr Janosch, was hilft gegen Langeweile im Alter?</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>14.90</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Janosch</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>geschenkbuecher</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Was hält jung? Und was macht man eigentlich so den lieben langen Tag, wenn das Arbeitsleben hinter einem liegt? Auf solche und viele andere große Fragen weiß niemand eine bessere Antwort als Herr Wondrak. Er ist der Held der Erwachsenenwelt, den Janosch von 2013 bis 2019 für die Leserinnen des »ZEITmagazins« entworfen hat. Dieses besondere Geschenkbuch vereint die besten Zeichnungen mit humorvollen Fragen und Antworten rund um das Thema Rente und Ruhestand ein einzigartiges Geschenk für alle, die kurz vor dem Ruhestand stehen oder bereits mittendrin sind.</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>978-3-7423-2343-9</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>25.04.2023</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Breite 160 mm, Höhe 160 mm, Dicke 6 mmGewicht128 g</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>55797789</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Ffftsch und der Wirbelsturm</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>24.90</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Koller, Boni</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>kids bis11</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Auf dem Heimweg von der Schule lernt Leo die Ausserirdische Ffftsch kennen, die eine Schularbeit über das Wetter auf der Erde schreiben muss. Leo erklärt ihr Regen und Schnee, aber Ffftsch will unbedingt ein richtiges Gewitter erleben. Also gehen die beiden ins Fernsehstudio, um einen Meteorologen zu befragen. Als Ffftsch erfährt, dass in der Gegend von Miami ein Hurrikan wütet, packt sie Leo und den Fernsehmann Freddy in ihr Raumschiff und fliegt mit ihnen in den Sturm! Gemeinsam schaffen sie es, dem Hurrikan zu trotzen, und retten dabei die Besatzung eines Fischerboots aus grösster Not ...</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>978-3-85546-400-5</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Baeschlin</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>15.05.2023</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Breite 152 mm, Höhe 216 mm, Dicke 12 mmGewicht272 gIllustrationenMit Illustrationen in SW</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Die Insel der Orangenblüten - -</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>23.90</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Blum, Fiona</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>taschenbuch romane</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Sommer, Sonne, Italien! Die Trattoria Paradiso öffnet ihre Seeterrasse, und drei Schwestern finden das Glück.
+Auf einer kleinen malerischen Insel im Trasimeno-See ist die Trattoria Paradiso von Ernesto Peluso das Herzstück der Einwohner. Als Ernesto plötzlich stirbt, muss seine jüngste Tochter Greta das Lokal allein weiterführen. Sie ist wie ihr Vater eine begnadete Köchin, und zur großen Erleichterung der eingeschworenen Inselgemeinschaft scheint in der Trattoria alles so zu bleiben, wie es war. Der überraschende Tod des Vaters bringt jedoch auch Greta und ihre beiden älteren Schwestern Lorena und Gina, von denen sie sich längst entfremdet hat, wieder zusammen und konfrontiert sie mit ihrer lange verdrängten Vergangenheit. Und so müssen die drei so verschiedenen Frauen endlich ihrem großen Familiengeheimnis auf den Grund gehen: was in jener Nacht vor vielen Jahren geschah, als ihre Mutter spurlos verschwand ...</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>978-3-442-20643-8</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Taschenbuch</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Goldmann</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Originalausgabe</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Breite 136 mm, Höhe 207 mm, Dicke 36 mmGewicht476 g</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Treibholz</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>17.90</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>Pauly, Gisa</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Heyne Taschenb.</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>CHF 21.50</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>432 S.</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Deutsch</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Kartonierter Einband (Kt)</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>36066149</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>978-3-453-42579-8</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>Originalausgabe</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>Die Sylt-Saga</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>Brit, Kari und Alisia: drei Frauen und ihre Lebensträume - der dritte Band der großen Syltsaga
-Sylt, Gegenwart. Das berühmte Café und Hotel König Augustin wird mittlerweile von Kari geleitet, Brit hat sich aus dem Alltagsgeschäft zurückgezogen. Aber wie soll es weitergehen? Karis Tochter Alisia, die das Geschäft übernehmen soll, hat eine eigene Karriere: Sie ist ein gefragtes Model und erobert unter dem Namen "La Cappuccina" sämtliche Laufstege. Dann aber ändert sich alles, denn ihr begegnet die große Liebe. Dieser Mann scheint jedoch genau der Falsche zu sein...</t>
-        </is>
-      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>taschenbuch krimis</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Das Meer schwemmt jede Menge Fragen an
+Vor fünf Jahren wurde Sandra Lührsen des Mordes an ihrer Schwiegermutter schuldig gesprochen. Nun stellt sich heraus, dass eine Falschaussage zu dem Urteil führte. Was für ein Skandal! Die vermeintliche Mörderin muss freigesprochen werden und kehrt nach Sylt zurück. Wie zu erwarten, überschlagen sich die Spekulationen der Sylter - Mamma Carlotta jedenfalls steht auf Sandras Seite, welch schreckliches Schicksal die Arme durchleiden musste! Doch wer ist der wahre Mörder ihrer Schwiegermutter? Genau das soll Kommissar Erik Wolf jetzt herausfinden; kein leichtes Unterfangen nach so langer Zeit. Er ahnt natürlich nicht, dass es tatsächlich jemanden auf der Insel gibt, der mehr weiß und gute Gründe hat, zu schweigen ...
+Die Kult-Ermittlerin Mamma Carlotta ist auch in ihrem neuesten Fall wieder auf geheimer Verbrecherjagd und erlebt so manches Abenteuer.
+Mamma Carlottas 17. Fall auf Sylt! Diese Bände der Reihe sind bereits erschienen:
+Band 1: Die Tote am WattBand 2: GestrandetBand 3: Tod im DünengrasBand 4: Flammen im SandBand 5: InselzirkusBand 6: KüstennebelBand 7: KurschattenBand 8: StrandläuferBand 9: SonnendeckBand 10: GegenwindBand 11: VogelkojeBand 12: WellenbrecherBand 13: SturmflutBand 14: ZugvögelBand 15: LachmöweBand 16: Schwarze SchafeBand 17: Treibholz</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>978-3-492-31737-5</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Taschenbuch</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Piper</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>n-Nr.17</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Mein Kosmos-Buch Natur</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>35.90</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Oftring, Bärbel</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>kids sachbuch</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Das Standardwerk für Grundschulkinder.Warum werden im Herbst die Blätter bunt? Haben Tausendfüßer wirklich tausend Füße? Wohin ziehen die Zugvögel im Winter? "Mein Kosmos-Buch Natur" stellt mit über 800 Farbfotos und Zeichnungen unsere heimische Natur auf einmalig übersichtliche und verständliche Weise vor. Über 460 Tiere, Pflanzen und Pilze, die jeder kennen möchte, werden in ihren Lebensräumen vorgestellt. Die Steckbriefe wurden um eine "Lebensanzeige" ergänzt, die über den Bedrohungsgrad der jeweiligen Art informiert. Spannende Seiten mit modernen Infografiken zeigen ökologische Zusammenhänge, Biosysteme, Skurriles und Erstaunliches auf einen Blick. Zahlreiche Beobachtungstipps motivieren die Kinder, selbst aktiv zu werden.</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>978-3-440-17468-5</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Kosmos (Franckh-Kosmos)</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>1. A.</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Breite 216 mm, Höhe 300 mm, Dicke 24 mmGewicht1224 g</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Glücklich durch Frust</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>26.90</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Maas, Rüdiger</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>fachbuecher paedagogik erziehungsratgeber</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Viele Kinder sind es nicht mehr gewohnt mit Langeweile, Frust und Rückschlägen angemessen umzugehen. Sie hatten in ihrem jungen Leben auch kaum Gelegenheit, den Umgang damit zu üben, da ihre Eltern sie mit Ablenkungen, Annehmlichkeiten und Fürsorge überschütten, ihnen Hindernisse aus dem Weg räumen oder sie bei drohender Langeweile reflexartig bespaßen. Das tun sie im besten Glauben, "bedürfnisgerecht" zu erziehen und verwechseln dabei echte Bedürfnisse mit Wünschen oder umschiffen schlichtweg den Konflikt mit ihrem Kind. Gleichzeitig bekommen diese Kinder von ihren Eltern häufig eines nicht: ihre ungeteilte Zeit und Aufmerksamkeit, denn um diese Dinge konkurrieren sie mit dem Handydisplay und ziehen dabei häufig den Kürzeren.
+Mangelnde Frustrationstoleranz, eine gestörte Selbstregulationsfähigkeit, nicht altersgerecht ausgebildete soziale Kompetenzen und ein grundlegend geschwächtes Selbstbewusstsein sind die Folge.
+Der Psychologe und Generationenforscher Rüdiger Maas zeigt in seinem neuen Buch, wie es gelingt, sich in der Erziehung an wirklichen Bedürfnissen statt an Wünschen zu orientieren, damit Kinder sich ihres Werts und ihrer Fähigkeiten wieder bewusst werden und Eigenschaften wie Resilienz, die Fähigkeit zur Selbstregulation und ein stabiles Selbstvertrauen ausbilden. . Gleichzeitig erfahren Eltern, wie sie ihr Kind zu digitaler Kompetenz erziehen und ihr eigenes Medien-Verhalten positiv verändern können. So sind sie nicht nur gutes Vorbild, sondern auch ein verlässliches, wirklich verfügbares Gegenüber für ihre Kinder.</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>978-3-8338-8741-3</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Gräfe &amp; Unzer</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>04.05.2023</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>GU Partnerschaft &amp; Familie Einzeltitel</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Breite 138 mm, Höhe 210 mm, Dicke 18 mmGewicht302 g</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Lacroix und der traurige Champion von Roland-Garros</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>26.90</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Lépic, Alex</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>belletristik krimi</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Seit seine Frau Dominique für das Amt der Bürgermeisterin von Paris kandidiert, steht auch Lacroix im Rampenlicht. Dabei scheut der Commissaire nichts so sehr wie die Öffentlichkeit! Als Lacroix vor den neugierigen Blicken in sein Stammbistro flieht, tritt ein noch viel berühmterer Mann durch die Tür: Éric Seignosse, siebenmaliger Gewinner der French Open und Präsident des französischen Tennisverbands. Er hat im Parisien über Lacroix gelesen und ist sicher: Nur der berühmteste Polizist von Paris kann ihm helfen. Seignosses neuestes Tenniswunderkind, Yannick Duc, steht an diesem Abend im Halbfinale von Roland-Garros, doch seit dem Morgen ist sein Sieg mehr als ungewiss: Ducs Talisman, ein Tennisball, ohne den er seit seiner Kindheit kein Match bestreitet, wurde aus seinem Spind entwendet. Wer will den Sieg des jungen Mannes verhindern? Hat einer von Ducs Kontrahenten den Glücksbringer gestohlen? Lacroix taucht tief ein in die Geheimnisse des Tennissports, und Roland-Garros wird zum Match gegen einen großen Unbekannten.</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>978-3-311-12568-6</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>n-Nr.06</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>Breite 115 mm, Höhe 185 mm, Dicke 18 mm</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>